<commit_message>
added colourmap option to the plotting methods, added two docstrings
</commit_message>
<xml_diff>
--- a/Example data/test_output/NW13-33/clustering_stats.xlsx
+++ b/Example data/test_output/NW13-33/clustering_stats.xlsx
@@ -501,62 +501,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>27.495670955368947</t>
+          <t>7.282596530498042</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42.240005958254976</t>
+          <t>5.781538162088514</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.5872791256260825</t>
+          <t>4.480681735237585</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>836.2181000614445</t>
+          <t>9.1650568112698</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6.68304876459307</t>
+          <t>16.34000389284932</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4.614733647383023</t>
+          <t>0.444575557772317</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>37.733479807101496</t>
+          <t>5.442142526945816</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.5877073752024876</t>
+          <t>0.34236393275102794</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.095406557804383</t>
+          <t>0.7392034257074037</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.5280782765747482</t>
+          <t>0.23469015352424516</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>91.61053493957957</t>
+          <t>365.5951801659327</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>20.969761855996424</t>
+          <t>3.688888348215372</t>
         </is>
       </c>
     </row>
@@ -568,37 +568,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>27.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>34.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>6.0</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>881.0</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>38.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -618,12 +618,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>90.0</t>
+          <t>371.0</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>2.0</t>
         </is>
       </c>
     </row>
@@ -635,62 +635,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8.463186096193096</t>
+          <t>6.613682824170445</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>23.40109661914032</t>
+          <t>7.623740468330191</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.228632251950337</t>
+          <t>3.4226105097685484</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>166.98744425526297</t>
+          <t>27.307347550654605</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>15.689379570484268</t>
+          <t>22.792932057387993</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2.6978086633512914</t>
+          <t>0.843167504192013</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>12.878313930994016</t>
+          <t>3.5695826461722833</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.038603609950089</t>
+          <t>0.7478333125748428</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1.7082596463593163</t>
+          <t>1.0850605078477533</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1.0203982815940151</t>
+          <t>0.6511594519664378</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>18.30426029197649</t>
+          <t>52.93952991411122</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>48.288108560648034</t>
+          <t>13.677411131985362</t>
         </is>
       </c>
     </row>
@@ -788,62 +788,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>33.48023137812056</t>
+          <t>27.502658091378862</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>22.886188349908668</t>
+          <t>42.29818952377412</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4.35906230972194</t>
+          <t>6.588023718353842</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>14.31948447331033</t>
+          <t>835.7779843116845</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>131.2935812867871</t>
+          <t>6.700016729246441</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.5507966308098234</t>
+          <t>4.611890776608796</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>4.420154252080374</t>
+          <t>37.70300940555411</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.7201288816724173</t>
+          <t>0.5876891334250344</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.7879795007103714</t>
+          <t>1.0962303431354326</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.49410391719098845</t>
+          <t>0.5282724264842559</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>202.2849502740004</t>
+          <t>91.62814602773338</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>6.677156484676273</t>
+          <t>20.995074166325885</t>
         </is>
       </c>
     </row>
@@ -855,62 +855,62 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>33.0</t>
+          <t>27.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>34.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>881.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>134.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>38.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>201.0</t>
+          <t>90.0</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -922,62 +922,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8.054719807065256</t>
+          <t>8.471896100075787</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.203068009288055</t>
+          <t>23.44563823844928</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2.9148400373373047</t>
+          <t>4.2286670519098335</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>39.54135870196029</t>
+          <t>167.27674092106656</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>31.48587853933173</t>
+          <t>15.702477935075995</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.9770750426530831</t>
+          <t>2.6972846188767354</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2.9325510445243794</t>
+          <t>12.891375396998088</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.0751358675922742</t>
+          <t>1.038487814575872</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1.1329200463969824</t>
+          <t>1.7098754430913825</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1.016873944995297</t>
+          <t>1.0203467215766961</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>30.833074854535912</t>
+          <t>18.32338408567439</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>20.865300889223086</t>
+          <t>48.343301809248224</t>
         </is>
       </c>
     </row>
@@ -1075,62 +1075,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>43.836846681806286</t>
+          <t>43.851359460441685</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>64.30899175200291</t>
+          <t>64.27876334316551</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5.243607169088161</t>
+          <t>5.2403586913344435</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>139.87109655306324</t>
+          <t>139.1541088075457</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>12.475277114129655</t>
+          <t>12.488577489667762</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.9161861666652596</t>
+          <t>0.9128204261361236</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>7.906047124175833</t>
+          <t>7.886755297120496</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1.2604324077904316</t>
+          <t>1.2618936941657721</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.1262526065190412</t>
+          <t>1.1254489980476508</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.5102276852422479</t>
+          <t>0.5101209442270472</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>144.3059863405739</t>
+          <t>144.38923587927553</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>16.453724261943556</t>
+          <t>16.423769639702837</t>
         </is>
       </c>
     </row>
@@ -1209,62 +1209,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>29.973326780005802</t>
+          <t>29.98430820139444</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25.71032063215518</t>
+          <t>25.709350816380173</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.360662597948324</t>
+          <t>3.358139673177194</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>205.3963035654524</t>
+          <t>204.75541249227928</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>17.58353812680841</t>
+          <t>17.612760094192097</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1.2817021448822097</t>
+          <t>1.278447020542331</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>6.256004619599703</t>
+          <t>6.238340409724313</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.4738537451568543</t>
+          <t>1.4743177611990907</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1.582015278801264</t>
+          <t>1.5800679571773546</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1.006285947630915</t>
+          <t>1.006556612774136</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>55.937295260992265</t>
+          <t>55.94992044745402</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>48.55716367666969</t>
+          <t>48.51404965459006</t>
         </is>
       </c>
     </row>
@@ -1362,62 +1362,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25.215686274509803</t>
+          <t>33.48029741663706</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>43.72549019607843</t>
+          <t>22.882941684007513</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11.594771241830065</t>
+          <t>4.359163579150383</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>357.6884531590414</t>
+          <t>14.319788864639902</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>12.285403050108933</t>
+          <t>131.31078515962037</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2.4052287581699345</t>
+          <t>0.5508653504542456</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>18.583877995642702</t>
+          <t>4.4200172562553925</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.6993464052287581</t>
+          <t>0.7197584124245039</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>61.09803921568628</t>
+          <t>0.7879409227021266</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>4.734204793028322</t>
+          <t>0.49404659188955996</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>100.50544662309368</t>
+          <t>202.28590062427043</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>29.38562091503268</t>
+          <t>6.676988275897071</t>
         </is>
       </c>
     </row>
@@ -1429,39 +1429,39 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>33.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>22.0</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>29.0</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>7.0</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>344.0</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>134.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>16.0</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>0.0</t>
@@ -1469,22 +1469,22 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>51.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>201.0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>4.0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>95.0</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -1496,62 +1496,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>18.13527281167459</t>
+          <t>8.054178510332747</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>59.428898066624996</t>
+          <t>8.19950698330753</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17.32670986139239</t>
+          <t>2.914992328963089</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>261.13629046500813</t>
+          <t>39.53602417091528</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>22.455359356629586</t>
+          <t>31.468683574142656</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2.365615826255409</t>
+          <t>0.9771269502374855</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>12.938561093671023</t>
+          <t>2.9320902069128394</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.0831546397838743</t>
+          <t>1.0748144066457963</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>32.964779125939735</t>
+          <t>1.1329384129121685</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>7.835950471543475</t>
+          <t>1.0167318608464533</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>47.64352782650311</t>
+          <t>30.82779675048748</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>82.91264722544065</t>
+          <t>20.863991565936153</t>
         </is>
       </c>
     </row>
@@ -1649,62 +1649,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7.281840411683841</t>
+          <t>21.399349023535304</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5.7811165585956035</t>
+          <t>23.22709063595393</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4.480711444178153</t>
+          <t>6.696544817225838</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9.165549459239163</t>
+          <t>445.7886830245368</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>16.33776566624898</t>
+          <t>16.0678517776665</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.44455528656066373</t>
+          <t>1.4201301952929395</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5.442085670141973</t>
+          <t>9.204556835252879</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.3423642623389579</t>
+          <t>0.6965448172258387</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.7391695762722175</t>
+          <t>1.1464697045568353</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.23467438776627453</t>
+          <t>1.6179268903355033</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>365.5975741797345</t>
+          <t>53.96795192789184</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>3.6888283312449057</t>
+          <t>909.2315973960941</t>
         </is>
       </c>
     </row>
@@ -1716,62 +1716,62 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>362.5</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>371.0</t>
+          <t>47.0</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>745.5</t>
         </is>
       </c>
     </row>
@@ -1783,62 +1783,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6.612771808914275</t>
+          <t>22.53495608928019</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7.623288339372183</t>
+          <t>21.774939246001217</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.4226611397301925</t>
+          <t>5.665615754924016</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>27.307972537180756</t>
+          <t>390.7573715199935</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>22.791345339356255</t>
+          <t>26.022161369986776</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.8431617852524255</t>
+          <t>1.8476677724554775</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>3.569642193758417</t>
+          <t>7.629894639161574</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.7478415347010676</t>
+          <t>1.2489567322361228</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1.0850621041067412</t>
+          <t>1.7568319479815502</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.6511411940277821</t>
+          <t>5.0940320820490195</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>52.93869930370531</t>
+          <t>42.73848197144495</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>13.677615011812433</t>
+          <t>455.53338372575394</t>
         </is>
       </c>
     </row>
@@ -1936,62 +1936,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21.399499374217772</t>
+          <t>25.215686274509803</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>23.226783479349187</t>
+          <t>43.72549019607843</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.696120150187735</t>
+          <t>11.594771241830065</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>445.8252816020025</t>
+          <t>357.6884531590414</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>16.064330413016272</t>
+          <t>12.285403050108933</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.4202753441802254</t>
+          <t>2.4052287581699345</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>9.207259073842303</t>
+          <t>18.583877995642702</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.6966207759699624</t>
+          <t>0.6993464052287581</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.146182728410513</t>
+          <t>61.09803921568628</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1.6180225281602003</t>
+          <t>4.734204793028322</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>53.96795994993742</t>
+          <t>100.50544662309368</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>909.1141426783479</t>
+          <t>29.38562091503268</t>
         </is>
       </c>
     </row>
@@ -2003,62 +2003,62 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>22.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>29.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>344.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>16.0</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>363.0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>51.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>47.0</t>
+          <t>95.0</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>745.0</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -2070,62 +2070,62 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22.532137521244675</t>
+          <t>18.13527281167459</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>21.772222455004773</t>
+          <t>59.428898066624996</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5.664970196279765</t>
+          <t>17.32670986139239</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>390.71530885973885</t>
+          <t>261.13629046500813</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>26.019856031612207</t>
+          <t>22.455359356629586</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1.847459284135523</t>
+          <t>2.365615826255409</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>7.630850852141193</t>
+          <t>12.938561093671023</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.2488096340101102</t>
+          <t>1.0831546397838743</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1.7567056783087749</t>
+          <t>32.964779125939735</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>5.093398077360695</t>
+          <t>7.835950471543475</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>42.733132643187766</t>
+          <t>47.64352782650311</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>455.5368489636038</t>
+          <t>82.91264722544065</t>
         </is>
       </c>
     </row>

</xml_diff>